<commit_message>
classe 2.0 electric boogaloo
</commit_message>
<xml_diff>
--- a/datenverarbeitung/FabrikVerbindung.xlsx
+++ b/datenverarbeitung/FabrikVerbindung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavio\Desktop\TUDa\Freedom Plan\ADP Digitaler Schatten\Code\datenverarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAE15FB-FED0-4BCF-8D9E-BA1F0EA3F538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8652EF2-40FA-449F-9610-0DA3A3B1C959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="262">
   <si>
     <t>id</t>
   </si>
@@ -821,6 +821,9 @@
   </si>
   <si>
     <t>FB2 (Empties)</t>
+  </si>
+  <si>
+    <t>process_name</t>
   </si>
 </sst>
 </file>
@@ -1213,9 +1216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1226,9 +1229,12 @@
     <col min="4" max="4" width="41.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="36.08984375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.08984375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="29.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1262,6 +1268,9 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="11">
@@ -1289,7 +1298,9 @@
         <v>132</v>
       </c>
       <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="L2" s="11" t="s">
+        <v>257</v>
+      </c>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
@@ -1321,7 +1332,9 @@
         <v>137</v>
       </c>
       <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="L3" s="11" t="s">
+        <v>257</v>
+      </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
     </row>
@@ -1351,7 +1364,9 @@
         <v>141</v>
       </c>
       <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="L4" s="12" t="s">
+        <v>258</v>
+      </c>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
     </row>
@@ -1381,7 +1396,9 @@
         <v>141</v>
       </c>
       <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="L5" s="12" t="s">
+        <v>258</v>
+      </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
     </row>
@@ -1413,7 +1430,9 @@
         <v>141</v>
       </c>
       <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="L6" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
@@ -1437,7 +1456,9 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="L7" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
@@ -1469,7 +1490,9 @@
         <v>141</v>
       </c>
       <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="L8" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
     </row>
@@ -1501,7 +1524,9 @@
         <v>155</v>
       </c>
       <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="L9" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
@@ -1533,7 +1558,9 @@
         <v>160</v>
       </c>
       <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
@@ -1565,7 +1592,9 @@
         <v>165</v>
       </c>
       <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="L11" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
@@ -1601,7 +1630,9 @@
         <v>97</v>
       </c>
       <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
     </row>
@@ -1637,7 +1668,9 @@
         <v>17</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="L13" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
     </row>
@@ -1673,7 +1706,9 @@
         <v>102</v>
       </c>
       <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="L14" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
@@ -1709,7 +1744,9 @@
         <v>107</v>
       </c>
       <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="L15" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
     </row>
@@ -1745,7 +1782,9 @@
         <v>112</v>
       </c>
       <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="L16" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
     </row>
@@ -1781,7 +1820,9 @@
         <v>117</v>
       </c>
       <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="L17" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
@@ -1817,7 +1858,9 @@
         <v>122</v>
       </c>
       <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+      <c r="L18" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
@@ -1851,7 +1894,9 @@
         <v>127</v>
       </c>
       <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="L19" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
@@ -1881,7 +1926,9 @@
         <v>186</v>
       </c>
       <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
     </row>
@@ -1911,7 +1958,9 @@
         <v>191</v>
       </c>
       <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+      <c r="L21" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
     </row>
@@ -1941,7 +1990,9 @@
         <v>193</v>
       </c>
       <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="L22" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
     </row>
@@ -1971,7 +2022,9 @@
         <v>198</v>
       </c>
       <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="L23" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
     </row>
@@ -2001,7 +2054,9 @@
         <v>203</v>
       </c>
       <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
     </row>
@@ -2031,7 +2086,9 @@
         <v>208</v>
       </c>
       <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="L25" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
     </row>
@@ -2061,7 +2118,9 @@
         <v>213</v>
       </c>
       <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="L26" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
     </row>
@@ -2091,7 +2150,9 @@
         <v>215</v>
       </c>
       <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
+      <c r="L27" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
     </row>
@@ -2121,7 +2182,9 @@
         <v>220</v>
       </c>
       <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="L28" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
     </row>
@@ -2151,7 +2214,9 @@
         <v>225</v>
       </c>
       <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="L29" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
     </row>
@@ -2173,7 +2238,9 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="L30" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
     </row>
@@ -2193,7 +2260,9 @@
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
+      <c r="L31" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
     </row>
@@ -2213,7 +2282,9 @@
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
+      <c r="L32" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
     </row>
@@ -2247,7 +2318,9 @@
         <v>92</v>
       </c>
       <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
+      <c r="L33" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
     </row>
@@ -2281,7 +2354,9 @@
         <v>69</v>
       </c>
       <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
+      <c r="L34" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
     </row>
@@ -2315,7 +2390,9 @@
         <v>61</v>
       </c>
       <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
+      <c r="L35" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
     </row>
@@ -2349,7 +2426,9 @@
         <v>45</v>
       </c>
       <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
+      <c r="L36" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
     </row>
@@ -2383,7 +2462,9 @@
         <v>37</v>
       </c>
       <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
+      <c r="L37" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
     </row>
@@ -2417,7 +2498,9 @@
         <v>84</v>
       </c>
       <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
     </row>
@@ -2451,7 +2534,9 @@
         <v>77</v>
       </c>
       <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
     </row>
@@ -2485,7 +2570,9 @@
         <v>53</v>
       </c>
       <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
+      <c r="L40" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
     </row>
@@ -2519,7 +2606,9 @@
         <v>25</v>
       </c>
       <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
+      <c r="L41" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
     </row>
@@ -2553,7 +2642,9 @@
         <v>29</v>
       </c>
       <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
+      <c r="L42" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
     </row>
@@ -2583,7 +2674,9 @@
         <v>141</v>
       </c>
       <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
+      <c r="L43" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
     </row>
@@ -2613,7 +2706,9 @@
         <v>141</v>
       </c>
       <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
+      <c r="L44" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
@@ -2641,7 +2736,9 @@
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
+      <c r="L45" s="12" t="s">
+        <v>253</v>
+      </c>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
     </row>
@@ -2673,7 +2770,9 @@
         <v>167</v>
       </c>
       <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
+      <c r="L46" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
     </row>
@@ -2705,7 +2804,9 @@
         <v>169</v>
       </c>
       <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
+      <c r="L47" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
     </row>
@@ -2737,7 +2838,9 @@
         <v>171</v>
       </c>
       <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
+      <c r="L48" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
     </row>
@@ -2769,7 +2872,9 @@
         <v>173</v>
       </c>
       <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
+      <c r="L49" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M49" s="11"/>
       <c r="N49" s="11"/>
     </row>
@@ -2801,7 +2906,9 @@
         <v>175</v>
       </c>
       <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
+      <c r="L50" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11"/>
     </row>
@@ -2833,7 +2940,9 @@
         <v>177</v>
       </c>
       <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
+      <c r="L51" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M51" s="11"/>
       <c r="N51" s="11"/>
     </row>
@@ -2865,7 +2974,9 @@
         <v>179</v>
       </c>
       <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
+      <c r="L52" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M52" s="11"/>
       <c r="N52" s="11"/>
     </row>
@@ -2897,7 +3008,9 @@
         <v>181</v>
       </c>
       <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
+      <c r="L53" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
     </row>
@@ -2914,8 +3027,8 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E30:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
começando a incluir bagulhos que eles querem
</commit_message>
<xml_diff>
--- a/datenverarbeitung/FabrikVerbindung.xlsx
+++ b/datenverarbeitung/FabrikVerbindung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavio\Desktop\TUDa\Freedom Plan\ADP Digitaler Schatten\Code\datenverarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED843169-EDB4-46E9-A06F-A86DEE8E392A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594BD7C3-BA32-4BCA-A4FE-A3761A6DA502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="308">
   <si>
     <t>id</t>
   </si>
@@ -87,9 +87,6 @@
     <t>aff183a4-42d8-4d8c-b21f-da6a796c6fda</t>
   </si>
   <si>
-    <t>(Fräsen or Sägen) then Waschen</t>
-  </si>
-  <si>
     <t>D40</t>
   </si>
   <si>
@@ -943,6 +940,15 @@
   </si>
   <si>
     <t>TransportLieferung</t>
+  </si>
+  <si>
+    <t>S001.M003.02.01, S001.M003.02.02, S001.M003.02.03</t>
+  </si>
+  <si>
+    <t>InitiallyUndefined</t>
+  </si>
+  <si>
+    <t>NOT_IMPORTANT</t>
   </si>
 </sst>
 </file>
@@ -1414,10 +1420,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
@@ -1427,11 +1433,11 @@
     <col min="3" max="3" width="36.26953125" customWidth="1"/>
     <col min="4" max="4" width="41.54296875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="46.08984375" customWidth="1"/>
     <col min="7" max="7" width="36.08984375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.08984375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.54296875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="6.54296875" customWidth="1"/>
     <col min="11" max="11" width="13.1796875" customWidth="1"/>
     <col min="12" max="12" width="29.08984375" customWidth="1"/>
     <col min="13" max="13" width="25.90625" customWidth="1"/>
@@ -1514,17 +1520,17 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
@@ -1533,41 +1539,41 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E3" s="1">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>20</v>
+        <v>307</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
@@ -1576,39 +1582,41 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>305</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
@@ -1617,39 +1625,41 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>305</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
@@ -1658,36 +1668,36 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1697,30 +1707,36 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1730,43 +1746,43 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E8" s="1">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N8" s="1">
         <v>4</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
@@ -1775,43 +1791,43 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N9" s="1">
         <v>8</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q9" s="1"/>
     </row>
@@ -1820,43 +1836,43 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N10" s="1">
         <v>4</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q10" s="1"/>
     </row>
@@ -1865,43 +1881,43 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E11" s="1">
         <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>53</v>
+        <v>306</v>
       </c>
       <c r="N11" s="1">
         <v>4</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="1"/>
     </row>
@@ -1910,47 +1926,47 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N12" s="3">
         <v>4</v>
       </c>
       <c r="O12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="Q12" s="3"/>
     </row>
@@ -1959,47 +1975,47 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="E13" s="4">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N13" s="3">
         <v>8</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
@@ -2008,47 +2024,47 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="3">
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N14" s="3">
         <v>4</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
@@ -2057,47 +2073,47 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="E15" s="3">
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N15" s="3">
         <v>8</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
@@ -2106,47 +2122,47 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="E16" s="3">
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N16" s="3">
         <v>4</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
@@ -2155,47 +2171,47 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="E17" s="3">
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N17" s="3">
         <v>8</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
@@ -2204,47 +2220,47 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="E18" s="3">
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N18" s="3">
         <v>4</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q18" s="3"/>
     </row>
@@ -2253,47 +2269,47 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="E19" s="3">
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N19" s="3">
         <v>8</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q19" s="3"/>
     </row>
@@ -2302,43 +2318,43 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E20" s="1">
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N20" s="1">
         <v>4</v>
       </c>
       <c r="O20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="Q20" s="1"/>
     </row>
@@ -2347,43 +2363,43 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="E21" s="1">
         <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N21" s="1">
         <v>4</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q21" s="1"/>
     </row>
@@ -2392,43 +2408,43 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N22" s="1">
         <v>8</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22" s="1"/>
     </row>
@@ -2437,43 +2453,43 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E23" s="1">
         <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N23" s="1">
         <v>4</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q23" s="1"/>
     </row>
@@ -2482,43 +2498,43 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N24" s="1">
         <v>4</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q24" s="1"/>
     </row>
@@ -2527,43 +2543,43 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N25" s="1">
         <v>4</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q25" s="1"/>
     </row>
@@ -2572,43 +2588,43 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="E26" s="1">
         <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N26" s="1">
         <v>4</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q26" s="1"/>
     </row>
@@ -2617,43 +2633,43 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E27" s="1">
         <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N27" s="1">
         <v>4</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q27" s="1"/>
     </row>
@@ -2662,43 +2678,43 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N28" s="1">
         <v>4</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q28" s="1"/>
     </row>
@@ -2707,43 +2723,43 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N29" s="1">
         <v>4</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q29" s="1"/>
     </row>
@@ -2752,10 +2768,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -2768,12 +2784,12 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -2783,7 +2799,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2795,12 +2811,12 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -2810,7 +2826,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2822,12 +2838,12 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2837,45 +2853,45 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="E33" s="2">
         <v>3</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="I33" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N33" s="2">
         <v>4</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q33" s="2"/>
     </row>
@@ -2884,45 +2900,45 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="E34" s="2">
         <v>3</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="I34" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N34" s="2">
         <v>4</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q34" s="2"/>
     </row>
@@ -2931,45 +2947,45 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>240</v>
       </c>
       <c r="E35" s="2">
         <v>3</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="I35" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N35" s="2">
         <v>4</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q35" s="2"/>
     </row>
@@ -2978,45 +2994,45 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="E36" s="9">
         <v>3</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="I36" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N36" s="2">
         <v>4</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q36" s="2"/>
     </row>
@@ -3025,45 +3041,45 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="E37" s="9">
         <v>3</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="I37" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N37" s="2">
         <v>4</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q37" s="2"/>
     </row>
@@ -3072,45 +3088,45 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E38" s="2">
         <v>3</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="I38" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N38" s="2">
         <v>8</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q38" s="2"/>
     </row>
@@ -3119,45 +3135,45 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C39" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="E39" s="2">
         <v>3</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="I39" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N39" s="2">
         <v>8</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q39" s="2"/>
     </row>
@@ -3166,45 +3182,45 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>260</v>
       </c>
       <c r="E40" s="9">
         <v>5</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="I40" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N40" s="2">
         <v>8</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q40" s="2"/>
     </row>
@@ -3213,45 +3229,45 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="E41" s="9">
         <v>3</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="I41" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N41" s="2">
         <v>8</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q41" s="2"/>
     </row>
@@ -3260,45 +3276,45 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="E42" s="9">
         <v>7</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="I42" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N42" s="2">
         <v>8</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q42" s="2"/>
     </row>
@@ -3307,32 +3323,32 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -3342,32 +3358,32 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -3377,30 +3393,30 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -3410,43 +3426,43 @@
         <v>44</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="E46" s="11">
         <v>5</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="J46" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>280</v>
       </c>
       <c r="K46" s="11"/>
       <c r="L46" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N46" s="11">
         <v>8</v>
       </c>
       <c r="O46" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P46" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q46" s="11"/>
     </row>
@@ -3455,43 +3471,43 @@
         <v>45</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="E47" s="11">
         <v>5</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>283</v>
-      </c>
-      <c r="J47" s="11" t="s">
-        <v>284</v>
       </c>
       <c r="K47" s="11"/>
       <c r="L47" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N47" s="11">
         <v>8</v>
       </c>
       <c r="O47" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P47" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q47" s="11"/>
     </row>
@@ -3500,43 +3516,43 @@
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C48" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="E48" s="11">
         <v>5</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="J48" s="11" t="s">
         <v>286</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>287</v>
       </c>
       <c r="K48" s="11"/>
       <c r="L48" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M48" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N48" s="11">
         <v>4</v>
       </c>
       <c r="O48" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P48" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q48" s="11"/>
     </row>
@@ -3545,43 +3561,43 @@
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C49" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="E49" s="11">
         <v>5</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="J49" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="K49" s="11"/>
       <c r="L49" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M49" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N49" s="11">
         <v>4</v>
       </c>
       <c r="O49" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P49" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q49" s="11"/>
     </row>
@@ -3590,43 +3606,43 @@
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="E50" s="11">
         <v>5</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>292</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>293</v>
       </c>
       <c r="K50" s="11"/>
       <c r="L50" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M50" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N50" s="11">
         <v>8</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q50" s="11"/>
     </row>
@@ -3635,43 +3651,43 @@
         <v>49</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="E51" s="11">
         <v>5</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="J51" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="J51" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="K51" s="11"/>
       <c r="L51" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M51" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N51" s="11">
         <v>8</v>
       </c>
       <c r="O51" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q51" s="11"/>
     </row>
@@ -3680,43 +3696,43 @@
         <v>50</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C52" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="E52" s="11">
         <v>5</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="J52" s="11" t="s">
         <v>298</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>299</v>
       </c>
       <c r="K52" s="11"/>
       <c r="L52" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M52" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N52" s="11">
         <v>4</v>
       </c>
       <c r="O52" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P52" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q52" s="11"/>
     </row>
@@ -3725,43 +3741,43 @@
         <v>51</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C53" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="E53" s="11">
         <v>5</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="J53" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="J53" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="K53" s="11"/>
       <c r="L53" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M53" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N53" s="11">
         <v>4</v>
       </c>
       <c r="O53" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q53" s="11"/>
     </row>

</xml_diff>

<commit_message>
bora matar essa porra por favor
</commit_message>
<xml_diff>
--- a/datenverarbeitung/FabrikVerbindung.xlsx
+++ b/datenverarbeitung/FabrikVerbindung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavio\Desktop\TUDa\Freedom Plan\ADP Digitaler Schatten\Code\datenverarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3C7FB-8AC7-421D-8217-721B8060ECAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DE1514-4A03-4EF4-8E94-BFC7D5A78A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1423,10 +1423,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
correções finais + quero morrer
</commit_message>
<xml_diff>
--- a/datenverarbeitung/FabrikVerbindung.xlsx
+++ b/datenverarbeitung/FabrikVerbindung.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavio\Desktop\TUDa\Freedom Plan\ADP Digitaler Schatten\Code\datenverarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DE1514-4A03-4EF4-8E94-BFC7D5A78A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699CB7B9-66CE-459A-B474-45E5685C44EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,12 +1421,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
@@ -1938,7 +1939,7 @@
         <v>76</v>
       </c>
       <c r="E12" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>77</v>
@@ -1987,7 +1988,7 @@
         <v>87</v>
       </c>
       <c r="E13" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>88</v>
@@ -2036,7 +2037,7 @@
         <v>97</v>
       </c>
       <c r="E14" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>98</v>
@@ -2085,7 +2086,7 @@
         <v>107</v>
       </c>
       <c r="E15" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>108</v>
@@ -2134,7 +2135,7 @@
         <v>117</v>
       </c>
       <c r="E16" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>118</v>
@@ -2183,7 +2184,7 @@
         <v>127</v>
       </c>
       <c r="E17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>128</v>
@@ -2232,7 +2233,7 @@
         <v>137</v>
       </c>
       <c r="E18" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>138</v>
@@ -2281,7 +2282,7 @@
         <v>147</v>
       </c>
       <c r="E19" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>148</v>
@@ -3208,7 +3209,7 @@
         <v>259</v>
       </c>
       <c r="E40" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>307</v>
@@ -3306,7 +3307,7 @@
         <v>267</v>
       </c>
       <c r="E42" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>307</v>

</xml_diff>